<commit_message>
update mitigator summary table
</commit_message>
<xml_diff>
--- a/summary_mitigators_table.xlsx
+++ b/summary_mitigators_table.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="34" documentId="8_{8A867626-2B52-4DB9-9FD2-4ACA95E94EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB53FCD9-6D85-40FE-9E13-4B68712979A0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20928" windowHeight="13800" xr2:uid="{C7C7E133-6540-4860-8BFB-5820B99056E7}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20928" windowHeight="13800" xr2:uid="{C7C7E133-6540-4860-8BFB-5820B99056E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -623,7 +623,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>